<commit_message>
chapter 13 one task done
</commit_message>
<xml_diff>
--- a/Chapter 13/hehe.xlsx
+++ b/Chapter 13/hehe.xlsx
@@ -350,7 +350,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -380,12 +380,6 @@
       <c r="H1" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="n">
-        <v>9</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -412,12 +406,6 @@
       <c r="H2" t="n">
         <v>1</v>
       </c>
-      <c r="I2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J2" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -444,12 +432,6 @@
       <c r="H3" t="n">
         <v>2</v>
       </c>
-      <c r="I3" t="n">
-        <v>2</v>
-      </c>
-      <c r="J3" t="n">
-        <v>2</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -476,12 +458,6 @@
       <c r="H4" t="n">
         <v>3</v>
       </c>
-      <c r="I4" t="n">
-        <v>3</v>
-      </c>
-      <c r="J4" t="n">
-        <v>3</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -508,12 +484,6 @@
       <c r="H5" t="n">
         <v>4</v>
       </c>
-      <c r="I5" t="n">
-        <v>4</v>
-      </c>
-      <c r="J5" t="n">
-        <v>4</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -540,12 +510,6 @@
       <c r="H6" t="n">
         <v>5</v>
       </c>
-      <c r="I6" t="n">
-        <v>5</v>
-      </c>
-      <c r="J6" t="n">
-        <v>5</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -572,12 +536,6 @@
       <c r="H7" t="n">
         <v>6</v>
       </c>
-      <c r="I7" t="n">
-        <v>6</v>
-      </c>
-      <c r="J7" t="n">
-        <v>6</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -603,76 +561,6 @@
       </c>
       <c r="H8" t="n">
         <v>7</v>
-      </c>
-      <c r="I8" t="n">
-        <v>7</v>
-      </c>
-      <c r="J8" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="n">
-        <v>8</v>
-      </c>
-      <c r="C9" t="n">
-        <v>8</v>
-      </c>
-      <c r="D9" t="n">
-        <v>8</v>
-      </c>
-      <c r="E9" t="n">
-        <v>8</v>
-      </c>
-      <c r="F9" t="n">
-        <v>8</v>
-      </c>
-      <c r="G9" t="n">
-        <v>8</v>
-      </c>
-      <c r="H9" t="n">
-        <v>8</v>
-      </c>
-      <c r="I9" t="n">
-        <v>8</v>
-      </c>
-      <c r="J9" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="n">
-        <v>9</v>
-      </c>
-      <c r="C10" t="n">
-        <v>9</v>
-      </c>
-      <c r="D10" t="n">
-        <v>9</v>
-      </c>
-      <c r="E10" t="n">
-        <v>9</v>
-      </c>
-      <c r="F10" t="n">
-        <v>9</v>
-      </c>
-      <c r="G10" t="n">
-        <v>9</v>
-      </c>
-      <c r="H10" t="n">
-        <v>9</v>
-      </c>
-      <c r="I10" t="n">
-        <v>9</v>
-      </c>
-      <c r="J10" t="n">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>